<commit_message>
removed thresholding and seems made the mask better
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>24bc57fa-ba23-4374-ac51-d434e6bf410f</t>
   </si>
@@ -57,6 +57,18 @@
   </si>
   <si>
     <t>a1ae3f44-5878-4d30-898d-4dd4b33f8cfa</t>
+  </si>
+  <si>
+    <t>ae7a28a6-02bc-4fa6-858b-ab1a6dc5a99f</t>
+  </si>
+  <si>
+    <t>b718aabc-6b8a-42c9-920e-3378addd5810</t>
+  </si>
+  <si>
+    <t>b817e6c4-4176-4211-a5c8-77b54fe2e04e</t>
+  </si>
+  <si>
+    <t>ba9b993d-c107-451f-9ba2-c6c8a79a18a2</t>
   </si>
 </sst>
 </file>
@@ -72,12 +84,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -92,8 +110,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -421,6 +443,9 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
+      <c r="B3">
+        <v>2920</v>
+      </c>
       <c r="C3">
         <v>713.66420273400001</v>
       </c>
@@ -435,6 +460,9 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
+      <c r="B4">
+        <v>2894</v>
+      </c>
       <c r="C4">
         <v>1028.91836803</v>
       </c>
@@ -446,8 +474,11 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="B5">
+        <v>3036</v>
       </c>
       <c r="C5">
         <v>1758.06012734</v>
@@ -463,6 +494,9 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
+      <c r="B6">
+        <v>4358</v>
+      </c>
       <c r="C6">
         <v>3965.49769861</v>
       </c>
@@ -471,6 +505,74 @@
       </c>
       <c r="E6">
         <v>3719.75808173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>2240</v>
+      </c>
+      <c r="C7">
+        <v>13210.1518799</v>
+      </c>
+      <c r="D7">
+        <v>2817.6672399600002</v>
+      </c>
+      <c r="E7">
+        <v>2334.6312535799998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>2947</v>
+      </c>
+      <c r="C8">
+        <v>2968.9877826299999</v>
+      </c>
+      <c r="D8">
+        <v>2456.5923633000002</v>
+      </c>
+      <c r="E8">
+        <v>2298.8461954200002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>2398</v>
+      </c>
+      <c r="C9">
+        <v>6963.0494914399997</v>
+      </c>
+      <c r="D9">
+        <v>5473.3906292499996</v>
+      </c>
+      <c r="E9">
+        <v>5382.5096341799999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>2390</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1475.1629000299999</v>
+      </c>
+      <c r="D10">
+        <v>1652.5141847699999</v>
+      </c>
+      <c r="E10">
+        <v>1475.1629000299999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished pipeline, need tuning and saving to csv, also need matching to cloud point
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>24bc57fa-ba23-4374-ac51-d434e6bf410f</t>
   </si>
@@ -69,16 +69,45 @@
   </si>
   <si>
     <t>ba9b993d-c107-451f-9ba2-c6c8a79a18a2</t>
+  </si>
+  <si>
+    <t>Height mask no thresholding</t>
+  </si>
+  <si>
+    <t>need to remove the trees!</t>
+  </si>
+  <si>
+    <t>need to remove the trees, a small one attached to the edge of the house</t>
+  </si>
+  <si>
+    <t>diff_nothresh</t>
+  </si>
+  <si>
+    <t>diff_height_only</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -110,12 +139,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,186 +425,299 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="5"/>
+    <col min="4" max="4" width="10.83203125" style="4"/>
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="5">
         <v>1898</v>
       </c>
       <c r="C2">
         <v>1775.1583715199999</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>2021.01283317</v>
       </c>
       <c r="E2">
         <v>1450.5662333499999</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F2" s="4">
+        <v>2315</v>
+      </c>
+      <c r="H2">
+        <f>(B2-F2)/B2</f>
+        <v>-0.21970495258166492</v>
+      </c>
+      <c r="I2">
+        <f>(C2-D2)/C2</f>
+        <v>-0.13849719866936963</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <v>2920</v>
       </c>
       <c r="C3">
         <v>713.66420273400001</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <v>1682.8610781699999</v>
       </c>
       <c r="E3">
         <v>713.66420273400001</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="4">
+        <v>3216</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H9" si="0">(B3-F3)/B3</f>
+        <v>-0.10136986301369863</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I9" si="1">(C3-D3)/C3</f>
+        <v>-1.35805729322428</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>2894</v>
       </c>
       <c r="C4">
         <v>1028.91836803</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <v>1940.5942206699999</v>
       </c>
       <c r="E4">
         <v>1028.91836803</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="4">
+        <v>3919</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>-0.35418106427090534</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>-0.88605265584433446</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="5">
         <v>3036</v>
       </c>
       <c r="C5">
         <v>1758.06012734</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <v>1877.26075704</v>
       </c>
       <c r="E5">
         <v>1758.06012734</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="4">
+        <v>2978</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>1.9104084321475624E-2</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>-6.7802362300517172E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="5">
         <v>4358</v>
       </c>
       <c r="C6">
         <v>3965.49769861</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="4">
         <v>3979.7331833200001</v>
       </c>
       <c r="E6">
         <v>3719.75808173</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="4">
+        <v>5147</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>-0.18104635153740248</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>-3.5898355747350221E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="5">
         <v>2240</v>
       </c>
       <c r="C7">
         <v>13210.1518799</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="4">
         <v>2817.6672399600002</v>
       </c>
       <c r="E7">
         <v>2334.6312535799998</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="4">
+        <v>2833.1513489600002</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>-0.26479970935714292</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>0.78670440237350781</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="5">
         <v>2947</v>
       </c>
       <c r="C8">
         <v>2968.9877826299999</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="4">
         <v>2456.5923633000002</v>
       </c>
       <c r="E8">
         <v>2298.8461954200002</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="4">
+        <v>2459.1692363500001</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0.16553470093315231</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>0.17258252874186891</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="5">
         <v>2398</v>
       </c>
       <c r="C9">
         <v>6963.0494914399997</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>5473.3906292499996</v>
       </c>
       <c r="E9">
-        <v>5382.5096341799999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+        <v>2341</v>
+      </c>
+      <c r="F9" s="4">
+        <v>5510.2977800899998</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>-1.2978723019557965</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>0.21393770991019193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="5">
         <v>2390</v>
       </c>
       <c r="C10" s="1">
         <v>1475.1629000299999</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="4">
         <v>1652.5141847699999</v>
       </c>
       <c r="E10">
         <v>1475.1629000299999</v>
+      </c>
+      <c r="F10" s="4">
+        <v>2384.3290610700001</v>
+      </c>
+      <c r="I10">
+        <f t="shared" ref="I3:I10" si="2">C10-D10</f>
+        <v>-177.35128473999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>